<commit_message>
Jared Goff Game Stats Excel Updated
</commit_message>
<xml_diff>
--- a/JaredGoffGameStats.xlsx
+++ b/JaredGoffGameStats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/natenystuen/Documents/University/Y2Spring2025/CS_364/Final_Project/FA_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{88559910-16CC-7746-80B6-26ECFCE6DDA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{6A776297-FD27-BF43-9722-41D52533C45F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{FFF52FF2-AB53-C640-8BED-7D582A3CCCBF}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>PassingCompletions</t>
   </si>
@@ -28,7 +28,7 @@
     <t>PassingAttempts</t>
   </si>
   <si>
-    <t>PassingYeards</t>
+    <t>PassingYards</t>
   </si>
   <si>
     <t>PassingTD</t>
@@ -59,6 +59,15 @@
   </si>
   <si>
     <t>Jared Goff Game States</t>
+  </si>
+  <si>
+    <t>Sacks</t>
+  </si>
+  <si>
+    <t>Tackles</t>
+  </si>
+  <si>
+    <t>Interceptions</t>
   </si>
 </sst>
 </file>
@@ -561,7 +570,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -572,6 +581,9 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -948,10 +960,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C94AC49B-133C-2D44-B997-0DFFD0992040}">
-  <dimension ref="A1:M20"/>
+  <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="157" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -959,13 +971,13 @@
     <col min="1" max="16384" width="15.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="4"/>
     </row>
-    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1002,8 +1014,17 @@
       <c r="L2" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>18</v>
       </c>
@@ -1040,8 +1061,17 @@
       <c r="L3" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M3" s="1">
+        <v>0</v>
+      </c>
+      <c r="N3" s="1">
+        <v>0</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>34</v>
       </c>
@@ -1078,8 +1108,17 @@
       <c r="L4" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M4" s="1">
+        <v>0</v>
+      </c>
+      <c r="N4" s="1">
+        <v>0</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>18</v>
       </c>
@@ -1116,8 +1155,17 @@
       <c r="L5" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M5" s="1">
+        <v>0</v>
+      </c>
+      <c r="N5" s="1">
+        <v>0</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>18</v>
       </c>
@@ -1154,8 +1202,17 @@
       <c r="L6" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M6" s="1">
+        <v>0</v>
+      </c>
+      <c r="N6" s="1">
+        <v>0</v>
+      </c>
+      <c r="O6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
         <v>18</v>
       </c>
@@ -1192,8 +1249,17 @@
       <c r="L7" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M7" s="1">
+        <v>0</v>
+      </c>
+      <c r="N7" s="1">
+        <v>0</v>
+      </c>
+      <c r="O7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>22</v>
       </c>
@@ -1230,8 +1296,17 @@
       <c r="L8" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M8" s="1">
+        <v>0</v>
+      </c>
+      <c r="N8" s="1">
+        <v>0</v>
+      </c>
+      <c r="O8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
         <v>12</v>
       </c>
@@ -1268,8 +1343,17 @@
       <c r="L9" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M9" s="1">
+        <v>0</v>
+      </c>
+      <c r="N9" s="1">
+        <v>0</v>
+      </c>
+      <c r="O9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>18</v>
       </c>
@@ -1306,8 +1390,17 @@
       <c r="L10" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M10" s="1">
+        <v>0</v>
+      </c>
+      <c r="N10" s="1">
+        <v>0</v>
+      </c>
+      <c r="O10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
         <v>15</v>
       </c>
@@ -1344,8 +1437,17 @@
       <c r="L11" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M11" s="1">
+        <v>0</v>
+      </c>
+      <c r="N11" s="1">
+        <v>0</v>
+      </c>
+      <c r="O11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
         <v>24</v>
       </c>
@@ -1382,8 +1484,17 @@
       <c r="L12" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M12" s="1">
+        <v>0</v>
+      </c>
+      <c r="N12" s="1">
+        <v>0</v>
+      </c>
+      <c r="O12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
         <v>26</v>
       </c>
@@ -1420,8 +1531,17 @@
       <c r="L13" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M13" s="1">
+        <v>0</v>
+      </c>
+      <c r="N13" s="1">
+        <v>0</v>
+      </c>
+      <c r="O13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
         <v>21</v>
       </c>
@@ -1458,8 +1578,17 @@
       <c r="L14" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M14" s="1">
+        <v>0</v>
+      </c>
+      <c r="N14" s="1">
+        <v>0</v>
+      </c>
+      <c r="O14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
         <v>32</v>
       </c>
@@ -1496,8 +1625,17 @@
       <c r="L15" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M15" s="1">
+        <v>0</v>
+      </c>
+      <c r="N15" s="1">
+        <v>0</v>
+      </c>
+      <c r="O15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="3">
         <v>38</v>
       </c>
@@ -1534,8 +1672,17 @@
       <c r="L16" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M16" s="1">
+        <v>0</v>
+      </c>
+      <c r="N16" s="1">
+        <v>0</v>
+      </c>
+      <c r="O16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="3">
         <v>23</v>
       </c>
@@ -1572,8 +1719,17 @@
       <c r="L17" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M17" s="1">
+        <v>0</v>
+      </c>
+      <c r="N17" s="1">
+        <v>0</v>
+      </c>
+      <c r="O17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="3">
         <v>26</v>
       </c>
@@ -1610,8 +1766,17 @@
       <c r="L18" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M18" s="1">
+        <v>0</v>
+      </c>
+      <c r="N18" s="1">
+        <v>0</v>
+      </c>
+      <c r="O18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="3">
         <v>27</v>
       </c>
@@ -1648,9 +1813,17 @@
       <c r="L19" s="3">
         <v>0</v>
       </c>
-      <c r="M19" s="3"/>
-    </row>
-    <row r="20" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M19" s="1">
+        <v>0</v>
+      </c>
+      <c r="N19" s="1">
+        <v>0</v>
+      </c>
+      <c r="O19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>

</xml_diff>